<commit_message>
Bug fixing in Delivery person wise sales and MTD target VS Sales charts
</commit_message>
<xml_diff>
--- a/AgingMaturedTable.xlsx
+++ b/AgingMaturedTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="99">
   <si>
     <t>Cust ID</t>
   </si>
@@ -43,235 +43,274 @@
     <t>Credit Amount</t>
   </si>
   <si>
-    <t>12010503377</t>
-  </si>
-  <si>
-    <t>12010139209</t>
-  </si>
-  <si>
-    <t>90000004505</t>
-  </si>
-  <si>
-    <t>90000024176</t>
-  </si>
-  <si>
-    <t>12010121314</t>
-  </si>
-  <si>
-    <t>12010146650</t>
-  </si>
-  <si>
-    <t>12010146469</t>
-  </si>
-  <si>
-    <t>12010146583</t>
-  </si>
-  <si>
-    <t>12010511596</t>
-  </si>
-  <si>
-    <t>12010146532</t>
-  </si>
-  <si>
-    <t>90000010931</t>
-  </si>
-  <si>
-    <t>Mr Alamgir Hossain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Popular Pharma B A Tobaco </t>
-  </si>
-  <si>
-    <t>Ganoswastho 24 Hours Pharmacy</t>
-  </si>
-  <si>
-    <t>Lab Aid Diagnostic</t>
-  </si>
-  <si>
-    <t>Mr Latifur Rahman</t>
-  </si>
-  <si>
-    <t>Mrs Simeen Hossain</t>
-  </si>
-  <si>
-    <t>Mr Arshad Waliur Rahman</t>
-  </si>
-  <si>
-    <t>Labaid Specialized Hospital</t>
-  </si>
-  <si>
-    <t>Priya Medicine Corner</t>
-  </si>
-  <si>
-    <t>Mr Saifur Rahman</t>
-  </si>
-  <si>
-    <t>MARIE STOPES BANGLADESH</t>
-  </si>
-  <si>
-    <t>National Distribution ManagerTDCL Gulshan TowerGulshan 02 Dh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 ShahbagShahbag Biponi BitanDhaka                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dhanmondi # 6                                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalabagan,Dhanmondi,Dhaka.                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChairmanTranscom GroupDhaka                                 </t>
-  </si>
-  <si>
-    <t>Managing Director And CEOTranscom Distribution Co LtdGulshan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DirectorTranscom Distribution CoLtdGulshan Tower            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outdoor Pharmacy House 6 Road 4Dhanmondi Dhaka              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jahangir Alam RoadSunibir HousingAdabor                     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DirectorTranscom LimitedGulshan Tower                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 No Staff Quarter,Dhanmondi,Dhaka                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">INST                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB12                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB51                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB31                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD52                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD64                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-262130     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-425808     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-626955     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-632536     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-685734     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-684072     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-777695     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-778690     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-781679     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-781933     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-782674     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-782281     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-677302     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-762186     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-784911     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-785629     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-763482     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-786980     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-789343     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKINV120-771106     </t>
-  </si>
-  <si>
-    <t>26 Oct 2017</t>
-  </si>
-  <si>
-    <t>04 Jun 2018</t>
-  </si>
-  <si>
-    <t>06 Mar 2019</t>
-  </si>
-  <si>
-    <t>13 Mar 2019</t>
-  </si>
-  <si>
-    <t>21 May 2019</t>
-  </si>
-  <si>
-    <t>19 May 2019</t>
-  </si>
-  <si>
-    <t>29 Sep 2019</t>
-  </si>
-  <si>
-    <t>30 Sep 2019</t>
-  </si>
-  <si>
-    <t>05 Oct 2019</t>
-  </si>
-  <si>
-    <t>06 Oct 2019</t>
+    <t>51052141032</t>
+  </si>
+  <si>
+    <t>51052100681</t>
+  </si>
+  <si>
+    <t>51011136788</t>
+  </si>
+  <si>
+    <t>51052000093</t>
+  </si>
+  <si>
+    <t>51052139088</t>
+  </si>
+  <si>
+    <t>51011118806</t>
+  </si>
+  <si>
+    <t>51052141880</t>
+  </si>
+  <si>
+    <t>51052140964</t>
+  </si>
+  <si>
+    <t>51011136342</t>
+  </si>
+  <si>
+    <t>90000023582</t>
+  </si>
+  <si>
+    <t>51052149966</t>
+  </si>
+  <si>
+    <t>51011136009</t>
+  </si>
+  <si>
+    <t>90000033171</t>
+  </si>
+  <si>
+    <t>Grameen G C Eye Hospital</t>
+  </si>
+  <si>
+    <t>Islamia Eye Hospital</t>
+  </si>
+  <si>
+    <t>Popular Pharmecy</t>
+  </si>
+  <si>
+    <t>Mamata Clinic</t>
+  </si>
+  <si>
+    <t>New Medicine Point</t>
+  </si>
+  <si>
+    <t>Salauddin Pharmacy</t>
+  </si>
+  <si>
+    <t>Square Clinic</t>
+  </si>
+  <si>
+    <t>Maa Medical Hall</t>
+  </si>
+  <si>
+    <t>Fatema Pharmacy</t>
+  </si>
+  <si>
+    <t>Jahanara hospital</t>
+  </si>
+  <si>
+    <t>Medicine House</t>
+  </si>
+  <si>
+    <t>Akhoan Pharmacy</t>
+  </si>
+  <si>
+    <t>Cadet College Barishal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rupatali Barisal                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogra Road Barisal                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sreenadi Madaripur Madaripur                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalibari Road Barisal                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sadar Road Barisal                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Near Dr Satish Pharmacy Charmuguria Bazar Madaripur         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC Office Jhalokathi                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awar Bazar Banaripara Barisal                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tekerhat                                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sutiakathi,Miarhat ,Swarupkhati.                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faraji Bazar Lalmohan Bhola                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostafapur Bus stand Madaripur                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sat Mail, Rohomotpur, Barishal                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM23                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM31                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM53                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM11                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM55                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB66                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM34                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM54                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM24                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB42                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM71                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BM35                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-185997     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-263385     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-284659     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-317802     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-343003     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-361875     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-373661     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-427574     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-445213     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-447812     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-436260     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-437534     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-438630     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-441739     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-442188     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-431100     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-461376     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-445954     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-462643     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKINV510-462645     </t>
+  </si>
+  <si>
+    <t>04 Jul 2018</t>
+  </si>
+  <si>
+    <t>08 Jan 2019</t>
+  </si>
+  <si>
+    <t>28 Feb 2019</t>
   </si>
   <si>
     <t>11 May 2019</t>
   </si>
   <si>
-    <t>09 Sep 2019</t>
-  </si>
-  <si>
-    <t>09 Oct 2019</t>
-  </si>
-  <si>
-    <t>10 Oct 2019</t>
-  </si>
-  <si>
-    <t>11 Sep 2019</t>
-  </si>
-  <si>
-    <t>12 Oct 2019</t>
-  </si>
-  <si>
-    <t>15 Oct 2019</t>
-  </si>
-  <si>
-    <t>21 Sep 2019</t>
+    <t>07 Jul 2019</t>
+  </si>
+  <si>
+    <t>19 Aug 2019</t>
+  </si>
+  <si>
+    <t>14 Sep 2019</t>
+  </si>
+  <si>
+    <t>15 Jan 2020</t>
+  </si>
+  <si>
+    <t>21 Feb 2020</t>
+  </si>
+  <si>
+    <t>26 Feb 2020</t>
+  </si>
+  <si>
+    <t>03 Feb 2020</t>
+  </si>
+  <si>
+    <t>05 Feb 2020</t>
+  </si>
+  <si>
+    <t>06 Feb 2020</t>
+  </si>
+  <si>
+    <t>14 Feb 2020</t>
+  </si>
+  <si>
+    <t>15 Feb 2020</t>
+  </si>
+  <si>
+    <t>22 Jan 2020</t>
+  </si>
+  <si>
+    <t>22 Mar 2020</t>
+  </si>
+  <si>
+    <t>22 Feb 2020</t>
+  </si>
+  <si>
+    <t>24 Mar 2020</t>
   </si>
 </sst>
 </file>
@@ -672,28 +711,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I2">
-        <v>875</v>
+        <v>548</v>
       </c>
       <c r="J2">
-        <v>360.83</v>
+        <v>7874.74</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -701,31 +740,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="H3">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I3">
-        <v>594</v>
+        <v>360</v>
       </c>
       <c r="J3">
-        <v>103170.62</v>
+        <v>5934.33</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -733,31 +772,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="H4">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I4">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="J4">
-        <v>7973.29</v>
+        <v>779.63</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -765,31 +804,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="H5">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I5">
-        <v>312</v>
+        <v>237</v>
       </c>
       <c r="J5">
-        <v>5055.5</v>
+        <v>926.33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -797,31 +836,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="H6">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I6">
-        <v>243</v>
+        <v>180</v>
       </c>
       <c r="J6">
-        <v>19494.77</v>
+        <v>2239.81</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -829,31 +868,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="H7">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="I7">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="J7">
-        <v>2738</v>
+        <v>477.79</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -861,31 +900,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I8">
-        <v>172</v>
+        <v>111</v>
       </c>
       <c r="J8">
-        <v>7787.95</v>
+        <v>6199.02</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -893,31 +932,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I9">
-        <v>171</v>
+        <v>78</v>
       </c>
       <c r="J9">
-        <v>4867.87</v>
+        <v>425.73</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -925,31 +964,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="J10">
-        <v>3141.25</v>
+        <v>17900</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -957,31 +996,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>166</v>
+        <v>66</v>
       </c>
       <c r="J11">
-        <v>2722.39</v>
+        <v>20178.18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -989,31 +1028,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I12">
-        <v>165</v>
+        <v>59</v>
       </c>
       <c r="J12">
-        <v>440.03</v>
+        <v>4759.87</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1021,31 +1060,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I13">
-        <v>165</v>
+        <v>57</v>
       </c>
       <c r="J13">
-        <v>220.02</v>
+        <v>6000.79</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1053,31 +1092,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="H14">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="I14">
-        <v>163</v>
+        <v>56</v>
       </c>
       <c r="J14">
-        <v>4050</v>
+        <v>4211.16</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1085,31 +1124,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="H15">
         <v>30</v>
       </c>
       <c r="I15">
-        <v>162</v>
+        <v>48</v>
       </c>
       <c r="J15">
-        <v>8101.44</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1117,31 +1156,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I16">
-        <v>162</v>
+        <v>47</v>
       </c>
       <c r="J16">
-        <v>6113.99</v>
+        <v>9241.139999999999</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1149,31 +1188,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I17">
-        <v>161</v>
+        <v>41</v>
       </c>
       <c r="J17">
-        <v>6580.53</v>
+        <v>59285.86</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1181,31 +1220,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H18">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="J18">
-        <v>792.0599999999999</v>
+        <v>7257.95</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1213,31 +1252,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I19">
-        <v>159</v>
+        <v>40</v>
       </c>
       <c r="J19">
-        <v>2966.7</v>
+        <v>10170.68</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1245,31 +1284,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>156</v>
+        <v>39</v>
       </c>
       <c r="J20">
-        <v>3694.75</v>
+        <v>16038.24</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1277,31 +1316,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="H21">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>150</v>
+        <v>39</v>
       </c>
       <c r="J21">
-        <v>3600</v>
+        <v>9268.360000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>